<commit_message>
R49 was changed to 4K7
</commit_message>
<xml_diff>
--- a/PCBA-Order_Files_for_JLPCB/FreeDSP_SMD_AB_plus_BOM1.xlsx
+++ b/PCBA-Order_Files_for_JLPCB/FreeDSP_SMD_AB_plus_BOM1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/iMacHDD/Users/HILO/Documents/KICAD_DATA/FreeDSP_SMD_AB_plus_i/0v2posted/PDF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/iMacHDD/Users/HILO/Documents/KICAD_DATA/FreeDSP_SMD_AB_plus_i/0v2posted/PCBA-Order_Files_for_JLPCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F8B21-D9F5-9844-9F36-3B5BDFDEF16E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C35BAA-73F5-CA4F-9F22-3877802B95C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28980" windowHeight="25760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="JL PCBA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="FreeDSP_SMD_AB_plus_BOM" localSheetId="0">'JL PCBA'!$B$1:$D$40</definedName>
+    <definedName name="FreeDSP_SMD_AB_plus_BOM" localSheetId="0">'JL PCBA'!$B$1:$D$41</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>D5</t>
   </si>
@@ -171,9 +171,6 @@
     <t>100R</t>
   </si>
   <si>
-    <t>R10,R25,R28,R41,R44,R49,R62</t>
-  </si>
-  <si>
     <t>47k</t>
   </si>
   <si>
@@ -527,6 +524,22 @@
   </si>
   <si>
     <t>R8,R9,R13,R14,R15,R16,R17,R48,R81,R93</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R10,R25,R28,R41,R44,R62</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4.7k</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R49</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C23162</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -534,7 +547,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -556,6 +569,22 @@
       <color theme="10"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -600,7 +629,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,6 +640,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -932,11 +967,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -958,7 +993,7 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -972,7 +1007,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -986,21 +1021,21 @@
         <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1014,7 +1049,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1028,7 +1063,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1036,27 +1071,27 @@
         <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1070,26 +1105,26 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1098,7 +1133,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1112,49 +1147,49 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1168,35 +1203,35 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1210,40 +1245,40 @@
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
@@ -1252,7 +1287,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1266,253 +1301,267 @@
         <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>94</v>
+      <c r="D25" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" t="s">
-        <v>119</v>
+      <c r="B41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F40">
-    <sortCondition ref="B1:B40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F41">
+    <sortCondition ref="B1:B41"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <hyperlinks>

</xml_diff>